<commit_message>
Cleaned up publication counts and cited by counts
Deleted many of the CF templates used for generating the results.
</commit_message>
<xml_diff>
--- a/CitedByCounts/ScopusCitedByCore.xlsx
+++ b/CitedByCounts/ScopusCitedByCore.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="5800" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>y uniq eids</t>
   </si>
@@ -62,6 +62,15 @@
   <si>
     <t>Core CB Updates</t>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
 </sst>
 </file>
 
@@ -70,7 +79,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -100,6 +109,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -118,7 +134,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -172,13 +188,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -205,6 +235,12 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -231,6 +267,12 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -563,10 +605,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O88"/>
+  <dimension ref="A1:O117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="O73" sqref="O73"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="G119" sqref="G119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4111,23 +4153,47 @@
       </c>
       <c r="B74">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>55300994</v>
       </c>
       <c r="C74">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1140</v>
       </c>
       <c r="D74">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1330</v>
       </c>
       <c r="E74">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>18516</v>
       </c>
       <c r="F74">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>68399</v>
+      </c>
+      <c r="H74">
+        <v>55301184</v>
+      </c>
+      <c r="I74">
+        <v>1330</v>
+      </c>
+      <c r="J74">
+        <v>19846</v>
+      </c>
+      <c r="K74">
+        <v>69729</v>
+      </c>
+      <c r="L74">
+        <v>55300994</v>
+      </c>
+      <c r="M74">
+        <v>1140</v>
+      </c>
+      <c r="N74">
+        <v>19656</v>
+      </c>
+      <c r="O74">
+        <v>69539</v>
       </c>
     </row>
     <row r="75" spans="1:15">
@@ -4136,23 +4202,47 @@
       </c>
       <c r="B75">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>55302145</v>
       </c>
       <c r="C75">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>2325</v>
       </c>
       <c r="D75">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1174</v>
       </c>
       <c r="E75">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>289526</v>
       </c>
       <c r="F75">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>211815</v>
+      </c>
+      <c r="H75">
+        <v>55300994</v>
+      </c>
+      <c r="I75">
+        <v>1174</v>
+      </c>
+      <c r="J75">
+        <v>290700</v>
+      </c>
+      <c r="K75">
+        <v>212989</v>
+      </c>
+      <c r="L75">
+        <v>55302145</v>
+      </c>
+      <c r="M75">
+        <v>2325</v>
+      </c>
+      <c r="N75">
+        <v>291851</v>
+      </c>
+      <c r="O75">
+        <v>214140</v>
       </c>
     </row>
     <row r="76" spans="1:15">
@@ -4161,23 +4251,47 @@
       </c>
       <c r="B76">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>55312630</v>
       </c>
       <c r="C76">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>12684</v>
       </c>
       <c r="D76">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>2199</v>
       </c>
       <c r="E76">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>76838</v>
       </c>
       <c r="F76">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>347521</v>
+      </c>
+      <c r="H76">
+        <v>55302145</v>
+      </c>
+      <c r="I76">
+        <v>2199</v>
+      </c>
+      <c r="J76">
+        <v>79037</v>
+      </c>
+      <c r="K76">
+        <v>349720</v>
+      </c>
+      <c r="L76">
+        <v>55312630</v>
+      </c>
+      <c r="M76">
+        <v>12684</v>
+      </c>
+      <c r="N76">
+        <v>89522</v>
+      </c>
+      <c r="O76">
+        <v>360205</v>
       </c>
     </row>
     <row r="77" spans="1:15">
@@ -4186,23 +4300,47 @@
       </c>
       <c r="B77">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>55317727</v>
       </c>
       <c r="C77">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>7934</v>
       </c>
       <c r="D77">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>2837</v>
       </c>
       <c r="E77">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>15998</v>
       </c>
       <c r="F77">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>65297</v>
+      </c>
+      <c r="H77">
+        <v>55312630</v>
+      </c>
+      <c r="I77">
+        <v>2837</v>
+      </c>
+      <c r="J77">
+        <v>18835</v>
+      </c>
+      <c r="K77">
+        <v>68134</v>
+      </c>
+      <c r="L77">
+        <v>55317727</v>
+      </c>
+      <c r="M77">
+        <v>7934</v>
+      </c>
+      <c r="N77">
+        <v>23932</v>
+      </c>
+      <c r="O77">
+        <v>73231</v>
       </c>
     </row>
     <row r="78" spans="1:15">
@@ -4211,23 +4349,47 @@
       </c>
       <c r="B78">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>55318636</v>
       </c>
       <c r="C78">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1115</v>
       </c>
       <c r="D78">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>206</v>
       </c>
       <c r="E78">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>58466</v>
       </c>
       <c r="F78">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>36877</v>
+      </c>
+      <c r="H78">
+        <v>55317727</v>
+      </c>
+      <c r="I78">
+        <v>206</v>
+      </c>
+      <c r="J78">
+        <v>58672</v>
+      </c>
+      <c r="K78">
+        <v>37083</v>
+      </c>
+      <c r="L78">
+        <v>55318636</v>
+      </c>
+      <c r="M78">
+        <v>1115</v>
+      </c>
+      <c r="N78">
+        <v>59581</v>
+      </c>
+      <c r="O78">
+        <v>37992</v>
       </c>
     </row>
     <row r="79" spans="1:15">
@@ -4236,23 +4398,47 @@
       </c>
       <c r="B79">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>55336470</v>
       </c>
       <c r="C79">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>18553</v>
       </c>
       <c r="D79">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>719</v>
       </c>
       <c r="E79">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>118047</v>
       </c>
       <c r="F79">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>170268</v>
+      </c>
+      <c r="H79">
+        <v>55318636</v>
+      </c>
+      <c r="I79">
+        <v>719</v>
+      </c>
+      <c r="J79">
+        <v>118766</v>
+      </c>
+      <c r="K79">
+        <v>170987</v>
+      </c>
+      <c r="L79">
+        <v>55336470</v>
+      </c>
+      <c r="M79">
+        <v>18553</v>
+      </c>
+      <c r="N79">
+        <v>136600</v>
+      </c>
+      <c r="O79">
+        <v>188821</v>
       </c>
     </row>
     <row r="80" spans="1:15">
@@ -4261,136 +4447,256 @@
       </c>
       <c r="B80">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>55336596</v>
       </c>
       <c r="C80">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>242</v>
       </c>
       <c r="D80">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="E80">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>285360</v>
       </c>
       <c r="F80">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+        <v>8582</v>
+      </c>
+      <c r="H80">
+        <v>55336470</v>
+      </c>
+      <c r="I80">
+        <v>116</v>
+      </c>
+      <c r="J80">
+        <v>285476</v>
+      </c>
+      <c r="K80">
+        <v>8698</v>
+      </c>
+      <c r="L80">
+        <v>55336596</v>
+      </c>
+      <c r="M80">
+        <v>242</v>
+      </c>
+      <c r="N80">
+        <v>285602</v>
+      </c>
+      <c r="O80">
+        <v>8824</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15">
       <c r="A81" s="2">
         <v>41663</v>
       </c>
       <c r="B81">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>55337818</v>
       </c>
       <c r="C81">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1432</v>
       </c>
       <c r="D81">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="E81">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>75451</v>
       </c>
       <c r="F81">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+        <v>42589</v>
+      </c>
+      <c r="H81">
+        <v>55336596</v>
+      </c>
+      <c r="I81">
+        <v>210</v>
+      </c>
+      <c r="J81">
+        <v>75661</v>
+      </c>
+      <c r="K81">
+        <v>42799</v>
+      </c>
+      <c r="L81">
+        <v>55337818</v>
+      </c>
+      <c r="M81">
+        <v>1432</v>
+      </c>
+      <c r="N81">
+        <v>76883</v>
+      </c>
+      <c r="O81">
+        <v>44021</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15">
       <c r="A82" s="2">
         <v>41664</v>
       </c>
       <c r="B82">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>55360779</v>
       </c>
       <c r="C82">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>25726</v>
       </c>
       <c r="D82">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>2765</v>
       </c>
       <c r="E82">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>166608</v>
       </c>
       <c r="F82">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+        <v>385201</v>
+      </c>
+      <c r="H82">
+        <v>55337818</v>
+      </c>
+      <c r="I82">
+        <v>2765</v>
+      </c>
+      <c r="J82">
+        <v>169373</v>
+      </c>
+      <c r="K82">
+        <v>387966</v>
+      </c>
+      <c r="L82">
+        <v>55360779</v>
+      </c>
+      <c r="M82">
+        <v>25726</v>
+      </c>
+      <c r="N82">
+        <v>192334</v>
+      </c>
+      <c r="O82">
+        <v>410927</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15">
       <c r="A83" s="2">
         <v>41665</v>
       </c>
       <c r="B83">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>55373139</v>
       </c>
       <c r="C83">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>17767</v>
       </c>
       <c r="D83">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>5407</v>
       </c>
       <c r="E83">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>179130</v>
       </c>
       <c r="F83">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+        <v>240308</v>
+      </c>
+      <c r="H83">
+        <v>55360779</v>
+      </c>
+      <c r="I83">
+        <v>5407</v>
+      </c>
+      <c r="J83">
+        <v>184537</v>
+      </c>
+      <c r="K83">
+        <v>245715</v>
+      </c>
+      <c r="L83">
+        <v>55373139</v>
+      </c>
+      <c r="M83">
+        <v>17767</v>
+      </c>
+      <c r="N83">
+        <v>196897</v>
+      </c>
+      <c r="O83">
+        <v>258075</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15">
       <c r="A84" s="2">
         <v>41666</v>
       </c>
       <c r="B84">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>55371743</v>
       </c>
       <c r="C84">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>416</v>
       </c>
       <c r="D84">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1812</v>
       </c>
       <c r="E84">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>20186</v>
       </c>
       <c r="F84">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
+        <v>15237</v>
+      </c>
+      <c r="H84">
+        <v>55373139</v>
+      </c>
+      <c r="I84">
+        <v>1812</v>
+      </c>
+      <c r="J84">
+        <v>21998</v>
+      </c>
+      <c r="K84">
+        <v>17049</v>
+      </c>
+      <c r="L84">
+        <v>55371743</v>
+      </c>
+      <c r="M84">
+        <v>416</v>
+      </c>
+      <c r="N84">
+        <v>20602</v>
+      </c>
+      <c r="O84">
+        <v>15653</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15">
       <c r="A85" s="2">
         <v>41667</v>
       </c>
       <c r="B85">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>55384014</v>
       </c>
       <c r="C85">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>12271</v>
       </c>
       <c r="D85">
         <f t="shared" si="12"/>
@@ -4398,45 +4704,93 @@
       </c>
       <c r="E85">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>110880</v>
       </c>
       <c r="F85">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
+        <v>170776</v>
+      </c>
+      <c r="H85">
+        <v>55371743</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>110880</v>
+      </c>
+      <c r="K85">
+        <v>170776</v>
+      </c>
+      <c r="L85">
+        <v>55384014</v>
+      </c>
+      <c r="M85">
+        <v>12271</v>
+      </c>
+      <c r="N85">
+        <v>123151</v>
+      </c>
+      <c r="O85">
+        <v>183047</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15">
       <c r="A86" s="2">
         <v>41668</v>
       </c>
       <c r="B86">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>55405454</v>
       </c>
       <c r="C86">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>22292</v>
       </c>
       <c r="D86">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>852</v>
       </c>
       <c r="E86">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>146212</v>
       </c>
       <c r="F86">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+        <v>683047</v>
+      </c>
+      <c r="H86">
+        <v>55384014</v>
+      </c>
+      <c r="I86">
+        <v>852</v>
+      </c>
+      <c r="J86">
+        <v>147064</v>
+      </c>
+      <c r="K86">
+        <v>683899</v>
+      </c>
+      <c r="L86">
+        <v>55405454</v>
+      </c>
+      <c r="M86">
+        <v>22292</v>
+      </c>
+      <c r="N86">
+        <v>168504</v>
+      </c>
+      <c r="O86">
+        <v>705339</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15">
       <c r="A87" s="2">
         <v>41669</v>
       </c>
       <c r="B87">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>55405397</v>
       </c>
       <c r="C87">
         <f t="shared" si="11"/>
@@ -4444,7 +4798,7 @@
       </c>
       <c r="D87">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="E87">
         <f t="shared" si="13"/>
@@ -4452,20 +4806,44 @@
       </c>
       <c r="F87">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
+        <v>824</v>
+      </c>
+      <c r="H87">
+        <v>55405454</v>
+      </c>
+      <c r="I87">
+        <v>57</v>
+      </c>
+      <c r="J87">
+        <v>57</v>
+      </c>
+      <c r="K87">
+        <v>881</v>
+      </c>
+      <c r="L87">
+        <v>55405397</v>
+      </c>
+      <c r="M87">
+        <v>0</v>
+      </c>
+      <c r="N87">
+        <v>0</v>
+      </c>
+      <c r="O87">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15">
       <c r="A88" s="2">
         <v>41670</v>
       </c>
       <c r="B88">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>55405399</v>
       </c>
       <c r="C88">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D88">
         <f t="shared" si="12"/>
@@ -4477,7 +4855,1273 @@
       </c>
       <c r="F88">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>93</v>
+      </c>
+      <c r="H88">
+        <v>55405397</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+      <c r="K88">
+        <v>93</v>
+      </c>
+      <c r="L88">
+        <v>55405399</v>
+      </c>
+      <c r="M88">
+        <v>2</v>
+      </c>
+      <c r="N88">
+        <v>2</v>
+      </c>
+      <c r="O88">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15">
+      <c r="A89" s="2">
+        <v>41671</v>
+      </c>
+      <c r="B89">
+        <f t="shared" ref="B89:B112" si="15">L89</f>
+        <v>55416799</v>
+      </c>
+      <c r="C89">
+        <f t="shared" ref="C89:C112" si="16">M89</f>
+        <v>11402</v>
+      </c>
+      <c r="D89">
+        <f t="shared" ref="D89:D112" si="17">I89</f>
+        <v>2</v>
+      </c>
+      <c r="E89">
+        <f t="shared" ref="E89:E112" si="18">N89-M89</f>
+        <v>185765</v>
+      </c>
+      <c r="F89">
+        <f t="shared" ref="F89:F112" si="19">O89-M89</f>
+        <v>173534</v>
+      </c>
+      <c r="H89">
+        <v>55405399</v>
+      </c>
+      <c r="I89">
+        <v>2</v>
+      </c>
+      <c r="J89">
+        <v>185767</v>
+      </c>
+      <c r="K89">
+        <v>173536</v>
+      </c>
+      <c r="L89">
+        <v>55416799</v>
+      </c>
+      <c r="M89">
+        <v>11402</v>
+      </c>
+      <c r="N89">
+        <v>197167</v>
+      </c>
+      <c r="O89">
+        <v>184936</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15">
+      <c r="A90" s="2">
+        <v>41672</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="15"/>
+        <v>55435486</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="16"/>
+        <v>20640</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="17"/>
+        <v>1953</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="18"/>
+        <v>293846</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="19"/>
+        <v>595148</v>
+      </c>
+      <c r="H90">
+        <v>55416799</v>
+      </c>
+      <c r="I90">
+        <v>1953</v>
+      </c>
+      <c r="J90">
+        <v>295799</v>
+      </c>
+      <c r="K90">
+        <v>597101</v>
+      </c>
+      <c r="L90">
+        <v>55435486</v>
+      </c>
+      <c r="M90">
+        <v>20640</v>
+      </c>
+      <c r="N90">
+        <v>314486</v>
+      </c>
+      <c r="O90">
+        <v>615788</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15">
+      <c r="A91" s="2">
+        <v>41673</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="15"/>
+        <v>55449703</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="16"/>
+        <v>20123</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="17"/>
+        <v>5906</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="18"/>
+        <v>110136</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="19"/>
+        <v>185599</v>
+      </c>
+      <c r="H91">
+        <v>55435486</v>
+      </c>
+      <c r="I91">
+        <v>5906</v>
+      </c>
+      <c r="J91">
+        <v>116042</v>
+      </c>
+      <c r="K91">
+        <v>191505</v>
+      </c>
+      <c r="L91">
+        <v>55449703</v>
+      </c>
+      <c r="M91">
+        <v>20123</v>
+      </c>
+      <c r="N91">
+        <v>130259</v>
+      </c>
+      <c r="O91">
+        <v>205722</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15">
+      <c r="A92" s="2">
+        <v>41674</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="15"/>
+        <v>55461346</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="16"/>
+        <v>12796</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="17"/>
+        <v>1153</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="18"/>
+        <v>191734</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="19"/>
+        <v>165289</v>
+      </c>
+      <c r="H92">
+        <v>55449703</v>
+      </c>
+      <c r="I92">
+        <v>1153</v>
+      </c>
+      <c r="J92">
+        <v>192887</v>
+      </c>
+      <c r="K92">
+        <v>166442</v>
+      </c>
+      <c r="L92">
+        <v>55461346</v>
+      </c>
+      <c r="M92">
+        <v>12796</v>
+      </c>
+      <c r="N92">
+        <v>204530</v>
+      </c>
+      <c r="O92">
+        <v>178085</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15">
+      <c r="A93" s="2">
+        <v>41675</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="15"/>
+        <v>55459172</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="16"/>
+        <v>2181</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="17"/>
+        <v>4355</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="18"/>
+        <v>237193</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="19"/>
+        <v>72790</v>
+      </c>
+      <c r="H93">
+        <v>55461346</v>
+      </c>
+      <c r="I93">
+        <v>4355</v>
+      </c>
+      <c r="J93">
+        <v>241548</v>
+      </c>
+      <c r="K93">
+        <v>77145</v>
+      </c>
+      <c r="L93">
+        <v>55459172</v>
+      </c>
+      <c r="M93">
+        <v>2181</v>
+      </c>
+      <c r="N93">
+        <v>239374</v>
+      </c>
+      <c r="O93">
+        <v>74971</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15">
+      <c r="A94" s="2">
+        <v>41676</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="15"/>
+        <v>55469211</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="16"/>
+        <v>12253</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="17"/>
+        <v>2214</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="18"/>
+        <v>20061</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="19"/>
+        <v>232253</v>
+      </c>
+      <c r="H94">
+        <v>55459172</v>
+      </c>
+      <c r="I94">
+        <v>2214</v>
+      </c>
+      <c r="J94">
+        <v>22275</v>
+      </c>
+      <c r="K94">
+        <v>234467</v>
+      </c>
+      <c r="L94">
+        <v>55469211</v>
+      </c>
+      <c r="M94">
+        <v>12253</v>
+      </c>
+      <c r="N94">
+        <v>32314</v>
+      </c>
+      <c r="O94">
+        <v>244506</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15">
+      <c r="A95" s="2">
+        <v>41677</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="15"/>
+        <v>55480394</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="16"/>
+        <v>15798</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="17"/>
+        <v>4615</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="18"/>
+        <v>156831</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="19"/>
+        <v>268612</v>
+      </c>
+      <c r="H95">
+        <v>55469211</v>
+      </c>
+      <c r="I95">
+        <v>4615</v>
+      </c>
+      <c r="J95">
+        <v>161446</v>
+      </c>
+      <c r="K95">
+        <v>273227</v>
+      </c>
+      <c r="L95">
+        <v>55480394</v>
+      </c>
+      <c r="M95">
+        <v>15798</v>
+      </c>
+      <c r="N95">
+        <v>172629</v>
+      </c>
+      <c r="O95">
+        <v>284410</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15">
+      <c r="A96" s="2">
+        <v>41678</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="15"/>
+        <v>55490490</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="16"/>
+        <v>15521</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="17"/>
+        <v>5425</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="18"/>
+        <v>154977</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="19"/>
+        <v>168818</v>
+      </c>
+      <c r="H96">
+        <v>55480394</v>
+      </c>
+      <c r="I96">
+        <v>5425</v>
+      </c>
+      <c r="J96">
+        <v>160402</v>
+      </c>
+      <c r="K96">
+        <v>174243</v>
+      </c>
+      <c r="L96">
+        <v>55490490</v>
+      </c>
+      <c r="M96">
+        <v>15521</v>
+      </c>
+      <c r="N96">
+        <v>170498</v>
+      </c>
+      <c r="O96">
+        <v>184339</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15">
+      <c r="A97" s="2">
+        <v>41679</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="15"/>
+        <v>55513629</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="16"/>
+        <v>26262</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="17"/>
+        <v>3123</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="18"/>
+        <v>157616</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="19"/>
+        <v>332848</v>
+      </c>
+      <c r="H97">
+        <v>55490490</v>
+      </c>
+      <c r="I97">
+        <v>3123</v>
+      </c>
+      <c r="J97">
+        <v>160739</v>
+      </c>
+      <c r="K97">
+        <v>335971</v>
+      </c>
+      <c r="L97">
+        <v>55513629</v>
+      </c>
+      <c r="M97">
+        <v>26262</v>
+      </c>
+      <c r="N97">
+        <v>183878</v>
+      </c>
+      <c r="O97">
+        <v>359110</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15">
+      <c r="A98" s="2">
+        <v>41680</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="15"/>
+        <v>55521256</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="16"/>
+        <v>7669</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="17"/>
+        <v>42</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="18"/>
+        <v>231464</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="19"/>
+        <v>248758</v>
+      </c>
+      <c r="H98">
+        <v>55513629</v>
+      </c>
+      <c r="I98">
+        <v>42</v>
+      </c>
+      <c r="J98">
+        <v>231506</v>
+      </c>
+      <c r="K98">
+        <v>248800</v>
+      </c>
+      <c r="L98">
+        <v>55521256</v>
+      </c>
+      <c r="M98">
+        <v>7669</v>
+      </c>
+      <c r="N98">
+        <v>239133</v>
+      </c>
+      <c r="O98">
+        <v>256427</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15">
+      <c r="A99" s="2">
+        <v>41681</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="15"/>
+        <v>55532580</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="16"/>
+        <v>15372</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="17"/>
+        <v>4048</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="18"/>
+        <v>217813</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="19"/>
+        <v>465067</v>
+      </c>
+      <c r="H99">
+        <v>55521256</v>
+      </c>
+      <c r="I99">
+        <v>4048</v>
+      </c>
+      <c r="J99">
+        <v>221861</v>
+      </c>
+      <c r="K99">
+        <v>469115</v>
+      </c>
+      <c r="L99">
+        <v>55532580</v>
+      </c>
+      <c r="M99">
+        <v>15372</v>
+      </c>
+      <c r="N99">
+        <v>233185</v>
+      </c>
+      <c r="O99">
+        <v>480439</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15">
+      <c r="A100" s="2">
+        <v>41682</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="15"/>
+        <v>55540007</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="16"/>
+        <v>10317</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="17"/>
+        <v>2890</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="18"/>
+        <v>153473</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="19"/>
+        <v>21640</v>
+      </c>
+      <c r="H100">
+        <v>55532580</v>
+      </c>
+      <c r="I100">
+        <v>2890</v>
+      </c>
+      <c r="J100">
+        <v>156363</v>
+      </c>
+      <c r="K100">
+        <v>24530</v>
+      </c>
+      <c r="L100">
+        <v>55540007</v>
+      </c>
+      <c r="M100">
+        <v>10317</v>
+      </c>
+      <c r="N100">
+        <v>163790</v>
+      </c>
+      <c r="O100">
+        <v>31957</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15">
+      <c r="A101" s="2">
+        <v>41683</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="15"/>
+        <v>55531374</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="17"/>
+        <v>8633</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="18"/>
+        <v>15628</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="19"/>
+        <v>6725</v>
+      </c>
+      <c r="H101">
+        <v>55540007</v>
+      </c>
+      <c r="I101">
+        <v>8633</v>
+      </c>
+      <c r="J101">
+        <v>24261</v>
+      </c>
+      <c r="K101">
+        <v>15358</v>
+      </c>
+      <c r="L101">
+        <v>55531374</v>
+      </c>
+      <c r="M101">
+        <v>0</v>
+      </c>
+      <c r="N101">
+        <v>15628</v>
+      </c>
+      <c r="O101">
+        <v>6725</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15">
+      <c r="A102" s="2">
+        <v>41684</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="15"/>
+        <v>55544627</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="16"/>
+        <v>15880</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="17"/>
+        <v>2627</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="18"/>
+        <v>172034</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="19"/>
+        <v>871010</v>
+      </c>
+      <c r="H102">
+        <v>55531374</v>
+      </c>
+      <c r="I102">
+        <v>2627</v>
+      </c>
+      <c r="J102">
+        <v>174661</v>
+      </c>
+      <c r="K102">
+        <v>873637</v>
+      </c>
+      <c r="L102">
+        <v>55544627</v>
+      </c>
+      <c r="M102">
+        <v>15880</v>
+      </c>
+      <c r="N102">
+        <v>187914</v>
+      </c>
+      <c r="O102">
+        <v>886890</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15">
+      <c r="A103" s="2">
+        <v>41685</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="15"/>
+        <v>55568540</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="16"/>
+        <v>26026</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="17"/>
+        <v>2113</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="18"/>
+        <v>286316</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="19"/>
+        <v>957127</v>
+      </c>
+      <c r="H103">
+        <v>55544627</v>
+      </c>
+      <c r="I103">
+        <v>2113</v>
+      </c>
+      <c r="J103">
+        <v>288429</v>
+      </c>
+      <c r="K103">
+        <v>959240</v>
+      </c>
+      <c r="L103">
+        <v>55568540</v>
+      </c>
+      <c r="M103">
+        <v>26026</v>
+      </c>
+      <c r="N103">
+        <v>312342</v>
+      </c>
+      <c r="O103">
+        <v>983153</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15">
+      <c r="A104" s="2">
+        <v>41686</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="15"/>
+        <v>55591619</v>
+      </c>
+      <c r="C104">
+        <f t="shared" si="16"/>
+        <v>25268</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="17"/>
+        <v>2189</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="18"/>
+        <v>127506</v>
+      </c>
+      <c r="F104">
+        <f t="shared" si="19"/>
+        <v>146869</v>
+      </c>
+      <c r="H104">
+        <v>55568540</v>
+      </c>
+      <c r="I104">
+        <v>2189</v>
+      </c>
+      <c r="J104">
+        <v>129695</v>
+      </c>
+      <c r="K104">
+        <v>149058</v>
+      </c>
+      <c r="L104">
+        <v>55591619</v>
+      </c>
+      <c r="M104">
+        <v>25268</v>
+      </c>
+      <c r="N104">
+        <v>152774</v>
+      </c>
+      <c r="O104">
+        <v>172137</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15">
+      <c r="A105" s="2">
+        <v>41687</v>
+      </c>
+      <c r="B105">
+        <f t="shared" si="15"/>
+        <v>55591992</v>
+      </c>
+      <c r="C105">
+        <f t="shared" si="16"/>
+        <v>702</v>
+      </c>
+      <c r="D105">
+        <f t="shared" si="17"/>
+        <v>329</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="18"/>
+        <v>65457</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="19"/>
+        <v>10389</v>
+      </c>
+      <c r="H105">
+        <v>55591619</v>
+      </c>
+      <c r="I105">
+        <v>329</v>
+      </c>
+      <c r="J105">
+        <v>65786</v>
+      </c>
+      <c r="K105">
+        <v>10718</v>
+      </c>
+      <c r="L105">
+        <v>55591992</v>
+      </c>
+      <c r="M105">
+        <v>702</v>
+      </c>
+      <c r="N105">
+        <v>66159</v>
+      </c>
+      <c r="O105">
+        <v>11091</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15">
+      <c r="A106" s="2">
+        <v>41688</v>
+      </c>
+      <c r="B106">
+        <f t="shared" si="15"/>
+        <v>55616660</v>
+      </c>
+      <c r="C106">
+        <f t="shared" si="16"/>
+        <v>26525</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="17"/>
+        <v>1857</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="18"/>
+        <v>141153</v>
+      </c>
+      <c r="F106">
+        <f t="shared" si="19"/>
+        <v>311179</v>
+      </c>
+      <c r="H106">
+        <v>55591992</v>
+      </c>
+      <c r="I106">
+        <v>1857</v>
+      </c>
+      <c r="J106">
+        <v>143010</v>
+      </c>
+      <c r="K106">
+        <v>313036</v>
+      </c>
+      <c r="L106">
+        <v>55616660</v>
+      </c>
+      <c r="M106">
+        <v>26525</v>
+      </c>
+      <c r="N106">
+        <v>167678</v>
+      </c>
+      <c r="O106">
+        <v>337704</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15">
+      <c r="A107" s="2">
+        <v>41689</v>
+      </c>
+      <c r="B107">
+        <f t="shared" si="15"/>
+        <v>55635261</v>
+      </c>
+      <c r="C107">
+        <f t="shared" si="16"/>
+        <v>21353</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="17"/>
+        <v>2752</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="18"/>
+        <v>208175</v>
+      </c>
+      <c r="F107">
+        <f t="shared" si="19"/>
+        <v>270044</v>
+      </c>
+      <c r="H107">
+        <v>55616660</v>
+      </c>
+      <c r="I107">
+        <v>2752</v>
+      </c>
+      <c r="J107">
+        <v>210927</v>
+      </c>
+      <c r="K107">
+        <v>272796</v>
+      </c>
+      <c r="L107">
+        <v>55635261</v>
+      </c>
+      <c r="M107">
+        <v>21353</v>
+      </c>
+      <c r="N107">
+        <v>229528</v>
+      </c>
+      <c r="O107">
+        <v>291397</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15">
+      <c r="A108" s="2">
+        <v>41690</v>
+      </c>
+      <c r="B108">
+        <f t="shared" si="15"/>
+        <v>55682268</v>
+      </c>
+      <c r="C108">
+        <f t="shared" si="16"/>
+        <v>48970</v>
+      </c>
+      <c r="D108">
+        <f t="shared" si="17"/>
+        <v>1963</v>
+      </c>
+      <c r="E108">
+        <f t="shared" si="18"/>
+        <v>75661</v>
+      </c>
+      <c r="F108">
+        <f t="shared" si="19"/>
+        <v>568071</v>
+      </c>
+      <c r="H108">
+        <v>55635261</v>
+      </c>
+      <c r="I108">
+        <v>1963</v>
+      </c>
+      <c r="J108">
+        <v>77624</v>
+      </c>
+      <c r="K108">
+        <v>570034</v>
+      </c>
+      <c r="L108">
+        <v>55682268</v>
+      </c>
+      <c r="M108">
+        <v>48970</v>
+      </c>
+      <c r="N108">
+        <v>124631</v>
+      </c>
+      <c r="O108">
+        <v>617041</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15">
+      <c r="A109" s="2">
+        <v>41691</v>
+      </c>
+      <c r="B109">
+        <f t="shared" si="15"/>
+        <v>55706099</v>
+      </c>
+      <c r="C109">
+        <f t="shared" si="16"/>
+        <v>23836</v>
+      </c>
+      <c r="D109">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="E109">
+        <f t="shared" si="18"/>
+        <v>22001</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="19"/>
+        <v>315964</v>
+      </c>
+      <c r="H109">
+        <v>55682268</v>
+      </c>
+      <c r="I109">
+        <v>5</v>
+      </c>
+      <c r="J109">
+        <v>22006</v>
+      </c>
+      <c r="K109">
+        <v>315969</v>
+      </c>
+      <c r="L109">
+        <v>55706099</v>
+      </c>
+      <c r="M109">
+        <v>23836</v>
+      </c>
+      <c r="N109">
+        <v>45837</v>
+      </c>
+      <c r="O109">
+        <v>339800</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15">
+      <c r="A110" s="2">
+        <v>41692</v>
+      </c>
+      <c r="B110">
+        <f t="shared" si="15"/>
+        <v>55706099</v>
+      </c>
+      <c r="C110">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="E110">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H110">
+        <v>55706099</v>
+      </c>
+      <c r="I110">
+        <v>0</v>
+      </c>
+      <c r="J110">
+        <v>0</v>
+      </c>
+      <c r="K110">
+        <v>0</v>
+      </c>
+      <c r="L110">
+        <v>55706099</v>
+      </c>
+      <c r="M110">
+        <v>0</v>
+      </c>
+      <c r="N110">
+        <v>0</v>
+      </c>
+      <c r="O110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15">
+      <c r="A111" s="2">
+        <v>41693</v>
+      </c>
+      <c r="B111">
+        <f t="shared" si="15"/>
+        <v>55706099</v>
+      </c>
+      <c r="C111">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="E111">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <v>55706099</v>
+      </c>
+      <c r="I111">
+        <v>0</v>
+      </c>
+      <c r="J111">
+        <v>0</v>
+      </c>
+      <c r="K111">
+        <v>0</v>
+      </c>
+      <c r="L111">
+        <v>55706099</v>
+      </c>
+      <c r="M111">
+        <v>0</v>
+      </c>
+      <c r="N111">
+        <v>0</v>
+      </c>
+      <c r="O111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15">
+      <c r="A112" s="2">
+        <v>41694</v>
+      </c>
+      <c r="B112">
+        <f t="shared" si="15"/>
+        <v>55743891</v>
+      </c>
+      <c r="C112">
+        <f t="shared" si="16"/>
+        <v>59467</v>
+      </c>
+      <c r="D112">
+        <f t="shared" si="17"/>
+        <v>21675</v>
+      </c>
+      <c r="E112">
+        <f t="shared" si="18"/>
+        <v>142437</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="19"/>
+        <v>942226</v>
+      </c>
+      <c r="H112">
+        <v>55706099</v>
+      </c>
+      <c r="I112">
+        <v>21675</v>
+      </c>
+      <c r="J112">
+        <v>164112</v>
+      </c>
+      <c r="K112">
+        <v>963901</v>
+      </c>
+      <c r="L112">
+        <v>55743891</v>
+      </c>
+      <c r="M112">
+        <v>59467</v>
+      </c>
+      <c r="N112">
+        <v>201904</v>
+      </c>
+      <c r="O112">
+        <v>1001693</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B115" s="3"/>
+      <c r="C115" s="4">
+        <f>AVERAGE(C3:C112)</f>
+        <v>12444.190909090908</v>
+      </c>
+      <c r="D115" s="4">
+        <f t="shared" ref="D115:F115" si="20">AVERAGE(D3:D112)</f>
+        <v>2278.0090909090909</v>
+      </c>
+      <c r="E115" s="4">
+        <f t="shared" si="20"/>
+        <v>87941.272727272721</v>
+      </c>
+      <c r="F115" s="4">
+        <f t="shared" si="20"/>
+        <v>215979.2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B116" s="3"/>
+      <c r="C116" s="3">
+        <f>MIN(C3:C112)</f>
+        <v>0</v>
+      </c>
+      <c r="D116" s="3">
+        <f t="shared" ref="D116:F116" si="21">MIN(D3:D112)</f>
+        <v>0</v>
+      </c>
+      <c r="E116" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="F116" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B117" s="3"/>
+      <c r="C117" s="3">
+        <f>MAX(C3:C112)</f>
+        <v>59467</v>
+      </c>
+      <c r="D117" s="3">
+        <f t="shared" ref="D117:F117" si="22">MAX(D3:D112)</f>
+        <v>34056</v>
+      </c>
+      <c r="E117" s="3">
+        <f t="shared" si="22"/>
+        <v>293846</v>
+      </c>
+      <c r="F117" s="3">
+        <f t="shared" si="22"/>
+        <v>957127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>